<commit_message>
ac should work for both d
</commit_message>
<xml_diff>
--- a/results/spreadsheets/Geo-Based Results - MAIN.xlsx
+++ b/results/spreadsheets/Geo-Based Results - MAIN.xlsx
@@ -11,13 +11,14 @@
     <sheet name="ux, ut, uxt" sheetId="1" r:id="rId2"/>
     <sheet name="f(ux,ut)" sheetId="6" r:id="rId3"/>
     <sheet name="Dual Info" sheetId="9" r:id="rId4"/>
-    <sheet name="Damping c" sheetId="18" r:id="rId5"/>
-    <sheet name="Hyperparameter" sheetId="11" r:id="rId6"/>
-    <sheet name="NN Complexity" sheetId="13" r:id="rId7"/>
-    <sheet name="Residual Based" sheetId="5" r:id="rId8"/>
-    <sheet name="Error-Based Resampling" sheetId="14" r:id="rId9"/>
-    <sheet name="SimpleCase_OneResample" sheetId="15" r:id="rId10"/>
-    <sheet name="Other Results" sheetId="12" r:id="rId11"/>
+    <sheet name="PDE Gradients" sheetId="19" r:id="rId5"/>
+    <sheet name="Damping c" sheetId="18" r:id="rId6"/>
+    <sheet name="Hyperparameter" sheetId="11" r:id="rId7"/>
+    <sheet name="NN Complexity" sheetId="13" r:id="rId8"/>
+    <sheet name="Residual Based" sheetId="5" r:id="rId9"/>
+    <sheet name="Error-Based Resampling" sheetId="14" r:id="rId10"/>
+    <sheet name="SimpleCase_OneResample" sheetId="15" r:id="rId11"/>
+    <sheet name="Other Results" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4271" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4308" uniqueCount="216">
   <si>
     <t>Parameters</t>
   </si>
@@ -654,6 +655,30 @@
   <si>
     <t>1 to 0 linearly</t>
   </si>
+  <si>
+    <t>pde_dt</t>
+  </si>
+  <si>
+    <t>Single measurement from slices</t>
+  </si>
+  <si>
+    <t>pde_dx</t>
+  </si>
+  <si>
+    <t>allencahn_uxt</t>
+  </si>
+  <si>
+    <t>ac_res</t>
+  </si>
+  <si>
+    <t>From test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>pde_dxt</t>
+  </si>
 </sst>
 </file>
 
@@ -1254,7 +1279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1523,6 +1548,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1531,12 +1562,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1559,6 +1584,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9309,6 +9339,377 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="A13:M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="177" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="179" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="187" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="189"/>
+      <c r="J1" s="181" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="181"/>
+      <c r="L1" s="182"/>
+      <c r="M1" s="183"/>
+    </row>
+    <row r="2" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="178"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="184"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="29">
+        <v>100</v>
+      </c>
+      <c r="J3" s="14">
+        <v>26418.6422233581</v>
+      </c>
+      <c r="K3" s="43">
+        <f>J3/3600</f>
+        <v>7.338511728710583</v>
+      </c>
+      <c r="L3" s="12">
+        <v>5.2729729219104403E-3</v>
+      </c>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="29">
+        <v>100</v>
+      </c>
+      <c r="J4" s="14">
+        <v>26503.885266065499</v>
+      </c>
+      <c r="K4" s="43">
+        <f>J4/3600</f>
+        <v>7.3621903516848608</v>
+      </c>
+      <c r="L4" s="12">
+        <v>3.1623405133801201E-3</v>
+      </c>
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="29">
+        <v>100</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="43">
+        <f t="shared" ref="K5:K12" si="0">J5/3600</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="21"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="29">
+        <v>100</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="21"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="29">
+        <v>100</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="21"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I8" s="29">
+        <v>100</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="12"/>
+      <c r="M8" s="21"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I9" s="29">
+        <v>100</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="21"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I10" s="29">
+        <v>100</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="21"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="29">
+        <v>100</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="21"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="29">
+        <v>100</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="21"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6">
+        <f>AVERAGE(J3:J12)</f>
+        <v>26461.2637447118</v>
+      </c>
+      <c r="K13" s="44">
+        <f>J13/3600</f>
+        <v>7.3503510401977223</v>
+      </c>
+      <c r="L13" s="19">
+        <f>AVERAGE(L3:L12)</f>
+        <v>4.2176567176452802E-3</v>
+      </c>
+      <c r="M13" s="147">
+        <f>_xlfn.STDEV.P(L3:L12)</f>
+        <v>1.0553162042651601E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -11088,7 +11489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
@@ -16000,8 +16401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U411"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23676,10 +24077,1556 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" style="204" customWidth="1"/>
+    <col min="7" max="7" width="4" style="204" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="177" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="179" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="187" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="189"/>
+      <c r="J1" s="181" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="181"/>
+      <c r="L1" s="182"/>
+      <c r="M1" s="183"/>
+      <c r="N1" s="185" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="181"/>
+      <c r="P1" s="186"/>
+    </row>
+    <row r="2" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="178"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="202" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="202" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="184"/>
+      <c r="N2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="170">
+        <v>1</v>
+      </c>
+      <c r="G3" s="170">
+        <v>1</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="29">
+        <v>100</v>
+      </c>
+      <c r="J3" s="14">
+        <v>27332.2717437744</v>
+      </c>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K13" si="0">J3/3600</f>
+        <v>7.5922977066039996</v>
+      </c>
+      <c r="L3" s="14">
+        <v>4.02411807233541E-4</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="13"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="170">
+        <v>1</v>
+      </c>
+      <c r="G4" s="170">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="29">
+        <v>100</v>
+      </c>
+      <c r="J4" s="14">
+        <v>29098.176594734101</v>
+      </c>
+      <c r="K4" s="11">
+        <f t="shared" si="0"/>
+        <v>8.0828268318705838</v>
+      </c>
+      <c r="L4" s="12">
+        <v>4.3600223158904601E-4</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="170">
+        <v>1</v>
+      </c>
+      <c r="G5" s="170">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="29">
+        <v>100</v>
+      </c>
+      <c r="J5" s="14">
+        <v>22901.337994098601</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>6.3614827761385007</v>
+      </c>
+      <c r="L5" s="12">
+        <v>2.4807203008524702E-3</v>
+      </c>
+      <c r="M5" s="21"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="203">
+        <v>1</v>
+      </c>
+      <c r="G6" s="203">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="29">
+        <v>100</v>
+      </c>
+      <c r="J6" s="14">
+        <v>19776.823683500199</v>
+      </c>
+      <c r="K6" s="11">
+        <f t="shared" si="0"/>
+        <v>5.4935621343056109</v>
+      </c>
+      <c r="L6" s="12">
+        <v>1.3984005232912701E-3</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="203">
+        <v>1</v>
+      </c>
+      <c r="G7" s="203">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="29">
+        <v>100</v>
+      </c>
+      <c r="J7" s="14">
+        <v>24638.326832771301</v>
+      </c>
+      <c r="K7" s="11">
+        <f t="shared" si="0"/>
+        <v>6.8439796757698055</v>
+      </c>
+      <c r="L7" s="12">
+        <v>5.3373184743441696E-3</v>
+      </c>
+      <c r="M7" s="21"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="13"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="203"/>
+      <c r="G8" s="203"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="12"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="13"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="13"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="170"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="170"/>
+      <c r="G11" s="170"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="170"/>
+      <c r="G12" s="170"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="171"/>
+      <c r="G13" s="171"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="26"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="170">
+        <v>1</v>
+      </c>
+      <c r="G14" s="170">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="29">
+        <v>100</v>
+      </c>
+      <c r="J14" s="14">
+        <v>23894.370086193001</v>
+      </c>
+      <c r="K14" s="11">
+        <f t="shared" ref="K14:K24" si="1">J14/3600</f>
+        <v>6.6373250239425001</v>
+      </c>
+      <c r="L14" s="12">
+        <v>6.1982571449062905E-4</v>
+      </c>
+      <c r="M14" s="21"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="13"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="14">
+        <v>24969.523813486001</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="1"/>
+        <v>6.9359788370794444</v>
+      </c>
+      <c r="L15" s="12">
+        <v>5.0474948268934398E-4</v>
+      </c>
+      <c r="M15" s="21"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="170"/>
+      <c r="G16" s="170"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="14">
+        <v>25092.658141612999</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" si="1"/>
+        <v>6.970182817114722</v>
+      </c>
+      <c r="L16" s="12">
+        <v>9.0492772475214396E-4</v>
+      </c>
+      <c r="M16" s="21"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="170"/>
+      <c r="G17" s="170"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="14">
+        <v>25549.048943281101</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>7.096958039800306</v>
+      </c>
+      <c r="L17" s="12">
+        <v>5.2124448440414703E-4</v>
+      </c>
+      <c r="M17" s="21"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="13"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="170"/>
+      <c r="G18" s="170"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="14">
+        <v>25690.8418810367</v>
+      </c>
+      <c r="K18" s="11">
+        <f t="shared" si="1"/>
+        <v>7.1363449669546393</v>
+      </c>
+      <c r="L18" s="12">
+        <v>7.2718660937565497E-4</v>
+      </c>
+      <c r="M18" s="21"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="13"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="170"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="14">
+        <v>26897.509712219198</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="1"/>
+        <v>7.4715304756164436</v>
+      </c>
+      <c r="L19" s="12">
+        <v>6.7884136133370104E-4</v>
+      </c>
+      <c r="M19" s="21"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="13"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="14">
+        <v>26980.367732286399</v>
+      </c>
+      <c r="K20" s="11">
+        <f t="shared" si="1"/>
+        <v>7.4945465923017771</v>
+      </c>
+      <c r="L20" s="12">
+        <v>7.9830686408568997E-4</v>
+      </c>
+      <c r="M20" s="21"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="13"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="170"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="14">
+        <v>27056.713521242102</v>
+      </c>
+      <c r="K21" s="11">
+        <f t="shared" si="1"/>
+        <v>7.515753755900584</v>
+      </c>
+      <c r="L21" s="12">
+        <v>3.93508723616712E-4</v>
+      </c>
+      <c r="M21" s="21"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="170"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="14">
+        <v>27168.8429129123</v>
+      </c>
+      <c r="K22" s="11">
+        <f t="shared" si="1"/>
+        <v>7.5469008091423051</v>
+      </c>
+      <c r="L22" s="12">
+        <v>3.8823112690458699E-4</v>
+      </c>
+      <c r="M22" s="21"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="13"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="170"/>
+      <c r="G23" s="170"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="14">
+        <v>29425.480413675301</v>
+      </c>
+      <c r="K23" s="11">
+        <f t="shared" si="1"/>
+        <v>8.173744559354251</v>
+      </c>
+      <c r="L23" s="12">
+        <v>3.6191253874001499E-4</v>
+      </c>
+      <c r="M23" s="45"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="171"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6">
+        <f>AVERAGE(J14:J23)</f>
+        <v>26272.535715794511</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="1"/>
+        <v>7.2979265877206974</v>
+      </c>
+      <c r="L24" s="7">
+        <f>AVERAGE(L14:L23)</f>
+        <v>5.898734630392623E-4</v>
+      </c>
+      <c r="M24" s="28">
+        <f>_xlfn.STDEV.P(L14:L23)</f>
+        <v>1.7706268644262122E-4</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="26"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="170">
+        <v>1</v>
+      </c>
+      <c r="G25" s="170">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I25" s="29">
+        <v>100</v>
+      </c>
+      <c r="J25" s="14">
+        <v>25861.4030008316</v>
+      </c>
+      <c r="K25" s="11">
+        <f t="shared" ref="K25:K35" si="2">J25/3600</f>
+        <v>7.1837230557865555</v>
+      </c>
+      <c r="L25" s="12">
+        <v>3.7520808934642601E-4</v>
+      </c>
+      <c r="M25" s="21"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="13"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="14">
+        <v>25969.3847777843</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="2"/>
+        <v>7.2137179938289719</v>
+      </c>
+      <c r="L26" s="12">
+        <v>4.5763252523216399E-4</v>
+      </c>
+      <c r="M26" s="21"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="13"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="14">
+        <v>26142.395240068399</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" si="2"/>
+        <v>7.2617764555745552</v>
+      </c>
+      <c r="L27" s="12">
+        <v>2.5082805389114603E-4</v>
+      </c>
+      <c r="M27" s="21"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="14">
+        <v>26342.536836385701</v>
+      </c>
+      <c r="K28" s="11">
+        <f t="shared" si="2"/>
+        <v>7.317371343440473</v>
+      </c>
+      <c r="L28" s="12">
+        <v>3.1877921428105399E-4</v>
+      </c>
+      <c r="M28" s="21"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="13"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="14">
+        <v>26570.197723865502</v>
+      </c>
+      <c r="K29" s="11">
+        <f t="shared" si="2"/>
+        <v>7.3806104788515281</v>
+      </c>
+      <c r="L29" s="12">
+        <v>3.0757220676953502E-4</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="13"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="170"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="14">
+        <v>26615.942201137499</v>
+      </c>
+      <c r="K30" s="11">
+        <f t="shared" si="2"/>
+        <v>7.3933172780937495</v>
+      </c>
+      <c r="L30" s="12">
+        <v>2.7757695628255198E-4</v>
+      </c>
+      <c r="M30" s="21"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="13"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="170"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="14">
+        <v>27004.829962253501</v>
+      </c>
+      <c r="K31" s="11">
+        <f t="shared" si="2"/>
+        <v>7.5013416561815278</v>
+      </c>
+      <c r="L31" s="12">
+        <v>3.1443345655480701E-4</v>
+      </c>
+      <c r="M31" s="21"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="170"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="14">
+        <v>27124.239351511002</v>
+      </c>
+      <c r="K32" s="11">
+        <f t="shared" si="2"/>
+        <v>7.5345109309752782</v>
+      </c>
+      <c r="L32" s="12">
+        <v>4.5581336259583498E-4</v>
+      </c>
+      <c r="M32" s="21"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="170"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="14">
+        <v>25971.5489666461</v>
+      </c>
+      <c r="K33" s="11">
+        <f t="shared" si="2"/>
+        <v>7.214319157401694</v>
+      </c>
+      <c r="L33" s="12">
+        <v>4.4935761042617001E-4</v>
+      </c>
+      <c r="M33" s="21"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="170"/>
+      <c r="G34" s="170"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="14">
+        <v>26841.9584550857</v>
+      </c>
+      <c r="K34" s="11">
+        <f t="shared" si="2"/>
+        <v>7.4560995708571385</v>
+      </c>
+      <c r="L34" s="12">
+        <v>4.2995612261558598E-4</v>
+      </c>
+      <c r="M34" s="45"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="171"/>
+      <c r="G35" s="171"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="6">
+        <f>AVERAGE(J25:J34)</f>
+        <v>26444.443651556932</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="2"/>
+        <v>7.3456787920991475</v>
+      </c>
+      <c r="L35" s="7">
+        <f>AVERAGE(L25:L34)</f>
+        <v>3.6371575979952757E-4</v>
+      </c>
+      <c r="M35" s="28">
+        <f>_xlfn.STDEV.P(L25:L34)</f>
+        <v>7.5445594870073333E-5</v>
+      </c>
+      <c r="N35" s="4"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="26"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="170">
+        <v>1</v>
+      </c>
+      <c r="G36" s="170">
+        <v>1</v>
+      </c>
+      <c r="H36" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I36" s="29">
+        <v>100</v>
+      </c>
+      <c r="J36" s="14">
+        <v>30767.0578615665</v>
+      </c>
+      <c r="K36" s="11">
+        <f t="shared" ref="K36:K46" si="3">J36/3600</f>
+        <v>8.5464049615462496</v>
+      </c>
+      <c r="L36" s="12">
+        <v>4.9728287803700697E-4</v>
+      </c>
+      <c r="M36" s="21"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="170"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="14">
+        <v>31946.541281700102</v>
+      </c>
+      <c r="K37" s="11">
+        <f t="shared" si="3"/>
+        <v>8.8740392449166947</v>
+      </c>
+      <c r="L37" s="12">
+        <v>3.4030986416986599E-4</v>
+      </c>
+      <c r="M37" s="21"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="170"/>
+      <c r="G38" s="170"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="14">
+        <v>34068.940382003697</v>
+      </c>
+      <c r="K38" s="11">
+        <f t="shared" si="3"/>
+        <v>9.4635945505565822</v>
+      </c>
+      <c r="L38" s="12">
+        <v>5.0905370104560002E-4</v>
+      </c>
+      <c r="M38" s="21"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="13"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="170"/>
+      <c r="G39" s="170"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="14">
+        <v>34113.913825511903</v>
+      </c>
+      <c r="K39" s="11">
+        <f t="shared" si="3"/>
+        <v>9.4760871737533066</v>
+      </c>
+      <c r="L39" s="12">
+        <v>4.09241297970116E-4</v>
+      </c>
+      <c r="M39" s="21"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="13"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="170"/>
+      <c r="G40" s="170"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="14">
+        <v>34667.414845705003</v>
+      </c>
+      <c r="K40" s="11">
+        <f t="shared" si="3"/>
+        <v>9.6298374571402778</v>
+      </c>
+      <c r="L40" s="12">
+        <v>5.99672307261172E-4</v>
+      </c>
+      <c r="M40" s="21"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="13"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="170"/>
+      <c r="G41" s="170"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="14">
+        <v>34814.871627569097</v>
+      </c>
+      <c r="K41" s="11">
+        <f t="shared" si="3"/>
+        <v>9.6707976743247492</v>
+      </c>
+      <c r="L41" s="12">
+        <v>4.8776025678569699E-4</v>
+      </c>
+      <c r="M41" s="21"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="13"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="170"/>
+      <c r="G42" s="170"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="14">
+        <v>37221.653472423503</v>
+      </c>
+      <c r="K42" s="11">
+        <f t="shared" si="3"/>
+        <v>10.339348186784306</v>
+      </c>
+      <c r="L42" s="12">
+        <v>5.7929808223234204E-4</v>
+      </c>
+      <c r="M42" s="21"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="13"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="170"/>
+      <c r="G43" s="170"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="14">
+        <v>37512.479700326898</v>
+      </c>
+      <c r="K43" s="11">
+        <f t="shared" si="3"/>
+        <v>10.420133250090805</v>
+      </c>
+      <c r="L43" s="12">
+        <v>4.2558901654724701E-4</v>
+      </c>
+      <c r="M43" s="21"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="13"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="170"/>
+      <c r="G44" s="170"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="14">
+        <v>37536.824683904597</v>
+      </c>
+      <c r="K44" s="11">
+        <f t="shared" si="3"/>
+        <v>10.426895745529055</v>
+      </c>
+      <c r="L44" s="12">
+        <v>5.2411692438330702E-4</v>
+      </c>
+      <c r="M44" s="21"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="13"/>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="170"/>
+      <c r="G45" s="170"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="14">
+        <v>37616.753091573701</v>
+      </c>
+      <c r="K45" s="11">
+        <f t="shared" si="3"/>
+        <v>10.449098080992695</v>
+      </c>
+      <c r="L45" s="12">
+        <v>5.6434925910362496E-4</v>
+      </c>
+      <c r="M45" s="45"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="13"/>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="171"/>
+      <c r="G46" s="171"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="6">
+        <f>AVERAGE(J36:J45)</f>
+        <v>35026.645077228502</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" si="3"/>
+        <v>9.7296236325634737</v>
+      </c>
+      <c r="L46" s="7">
+        <f>AVERAGE(L36:L45)</f>
+        <v>4.9366735875359794E-4</v>
+      </c>
+      <c r="M46" s="28">
+        <f>_xlfn.STDEV.P(L36:L45)</f>
+        <v>7.7497370226460458E-5</v>
+      </c>
+      <c r="N46" s="4"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="26"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="170"/>
+      <c r="G47" s="170"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="11">
+        <f t="shared" ref="K47:K57" si="4">J47/3600</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="12"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="13"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="170"/>
+      <c r="G48" s="170"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L48" s="12"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="13"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="170"/>
+      <c r="G49" s="170"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L49" s="12"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="13"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="170"/>
+      <c r="G50" s="170"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L50" s="12"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="13"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="170"/>
+      <c r="G51" s="170"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L51" s="12"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="13"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="170"/>
+      <c r="G52" s="170"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L52" s="12"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="13"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="170"/>
+      <c r="G53" s="170"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L53" s="12"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="13"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="170"/>
+      <c r="G54" s="170"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L54" s="12"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="13"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="170"/>
+      <c r="G55" s="170"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L55" s="12"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="13"/>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="170"/>
+      <c r="G56" s="170"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L56" s="12"/>
+      <c r="M56" s="45"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="13"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="171"/>
+      <c r="G57" s="171"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="6" t="e">
+        <f>AVERAGE(J47:J56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K57" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L57" s="7" t="e">
+        <f>AVERAGE(L47:L56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M57" s="28" t="e">
+        <f>_xlfn.STDEV.P(L47:L56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N57" s="4"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23715,7 +25662,7 @@
       </c>
       <c r="K1" s="181"/>
       <c r="L1" s="182"/>
-      <c r="M1" s="193" t="s">
+      <c r="M1" s="190" t="s">
         <v>196</v>
       </c>
     </row>
@@ -23752,10 +25699,10 @@
       <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="194"/>
+      <c r="M2" s="191"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="192" t="s">
         <v>194</v>
       </c>
       <c r="B3" s="11"/>
@@ -23793,7 +25740,7 @@
       <c r="M3" s="172"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="191"/>
+      <c r="A4" s="193"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
         <v>43</v>
@@ -23829,7 +25776,7 @@
       <c r="M4" s="173"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="191"/>
+      <c r="A5" s="193"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
         <v>43</v>
@@ -23865,7 +25812,7 @@
       <c r="M5" s="173"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="191"/>
+      <c r="A6" s="193"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
         <v>43</v>
@@ -23901,7 +25848,7 @@
       <c r="M6" s="173"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="191"/>
+      <c r="A7" s="193"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
         <v>43</v>
@@ -23937,7 +25884,7 @@
       <c r="M7" s="173"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="191"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
         <v>43</v>
@@ -23973,7 +25920,7 @@
       <c r="M8" s="173"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="191"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
         <v>43</v>
@@ -24009,7 +25956,7 @@
       <c r="M9" s="173"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="191"/>
+      <c r="A10" s="193"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
         <v>43</v>
@@ -24045,7 +25992,7 @@
       <c r="M10" s="173"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="191"/>
+      <c r="A11" s="193"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
         <v>43</v>
@@ -24081,7 +26028,7 @@
       <c r="M11" s="173"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="192"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
         <v>43</v>
@@ -24131,11 +26078,11 @@
         <v>24496.838576722093</v>
       </c>
       <c r="K13" s="171">
-        <f t="shared" ref="K13:L13" si="1">AVERAGE(K3:K12)</f>
+        <f>AVERAGE(K3:K12)</f>
         <v>6.8046773824228044</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(L3:L12)</f>
         <v>4.2417335326063013E-4</v>
       </c>
       <c r="M13" s="174">
@@ -24209,7 +26156,7 @@
         <v>23772.587995052301</v>
       </c>
       <c r="K15" s="170">
-        <f t="shared" ref="K15:K23" si="2">J15/3600</f>
+        <f t="shared" ref="K15:K23" si="1">J15/3600</f>
         <v>6.6034966652923055</v>
       </c>
       <c r="L15" s="16">
@@ -24245,7 +26192,7 @@
         <v>23892.356754302898</v>
       </c>
       <c r="K16" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.6367657650841387</v>
       </c>
       <c r="L16" s="16">
@@ -24281,7 +26228,7 @@
         <v>24219.448536396001</v>
       </c>
       <c r="K17" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.7276245934433341</v>
       </c>
       <c r="L17" s="16">
@@ -24317,7 +26264,7 @@
         <v>24544.848488807598</v>
       </c>
       <c r="K18" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.8180134691132217</v>
       </c>
       <c r="L18" s="16">
@@ -24353,7 +26300,7 @@
         <v>24638.225636720599</v>
       </c>
       <c r="K19" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.8439515657557219</v>
       </c>
       <c r="L19" s="16">
@@ -24389,7 +26336,7 @@
         <v>25836.401496648701</v>
       </c>
       <c r="K20" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.1767781935135284</v>
       </c>
       <c r="L20" s="16">
@@ -24425,7 +26372,7 @@
         <v>26034.256717443401</v>
       </c>
       <c r="K21" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.2317379770676116</v>
       </c>
       <c r="L21" s="16">
@@ -24461,7 +26408,7 @@
         <v>26096.073242664301</v>
       </c>
       <c r="K22" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.2489092340734169</v>
       </c>
       <c r="L22" s="16">
@@ -24497,7 +26444,7 @@
         <v>26476.973431825601</v>
       </c>
       <c r="K23" s="170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.3547148421737782</v>
       </c>
       <c r="L23" s="16">
@@ -24520,11 +26467,11 @@
         <v>24871.355987429561</v>
       </c>
       <c r="K24" s="171">
-        <f t="shared" ref="K24" si="3">AVERAGE(K14:K23)</f>
+        <f>AVERAGE(K14:K23)</f>
         <v>6.9087099965082119</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" ref="L24" si="4">AVERAGE(L14:L23)</f>
+        <f>AVERAGE(L14:L23)</f>
         <v>4.8643891877348411E-4</v>
       </c>
       <c r="M24" s="174">
@@ -24600,7 +26547,7 @@
         <v>11585.206646442401</v>
       </c>
       <c r="K26" s="170">
-        <f t="shared" ref="K26:K34" si="5">J26/3600</f>
+        <f t="shared" ref="K26:K34" si="2">J26/3600</f>
         <v>3.2181129573451113</v>
       </c>
       <c r="L26" s="23">
@@ -24636,7 +26583,7 @@
         <v>21605.314297437599</v>
       </c>
       <c r="K27" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.0014761937326666</v>
       </c>
       <c r="L27" s="23">
@@ -24672,7 +26619,7 @@
         <v>22616.563446521701</v>
       </c>
       <c r="K28" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.282378735144917</v>
       </c>
       <c r="L28" s="23">
@@ -24708,7 +26655,7 @@
         <v>22887.4088261127</v>
       </c>
       <c r="K29" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.3576135628090835</v>
       </c>
       <c r="L29" s="23">
@@ -24744,7 +26691,7 @@
         <v>23867.5247731208</v>
       </c>
       <c r="K30" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.6298679925335557</v>
       </c>
       <c r="L30" s="23">
@@ -24780,7 +26727,7 @@
         <v>23926.7122197151</v>
       </c>
       <c r="K31" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.6463089499208614</v>
       </c>
       <c r="L31" s="23">
@@ -24816,7 +26763,7 @@
         <v>24230.030735731099</v>
       </c>
       <c r="K32" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.7305640932586384</v>
       </c>
       <c r="L32" s="23">
@@ -24852,7 +26799,7 @@
         <v>24308.4595673084</v>
       </c>
       <c r="K33" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.7523498798078894</v>
       </c>
       <c r="L33" s="23">
@@ -24888,7 +26835,7 @@
         <v>27482.2962856292</v>
       </c>
       <c r="K34" s="170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>7.6339711904525558</v>
       </c>
       <c r="L34" s="25">
@@ -24911,11 +26858,11 @@
         <v>21398.890902233077</v>
       </c>
       <c r="K35" s="171">
-        <f t="shared" ref="K35" si="6">AVERAGE(K25:K34)</f>
+        <f>AVERAGE(K25:K34)</f>
         <v>5.9441363617314105</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" ref="L35" si="7">AVERAGE(L25:L34)</f>
+        <f>AVERAGE(L25:L34)</f>
         <v>4.9315371656823257E-4</v>
       </c>
       <c r="M35" s="174">
@@ -25088,11 +27035,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K46" s="171" t="e">
-        <f t="shared" ref="K46" si="8">AVERAGE(K36:K45)</f>
+        <f>AVERAGE(K36:K45)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L46" s="6" t="e">
-        <f t="shared" ref="L46" si="9">AVERAGE(L36:L45)</f>
+        <f>AVERAGE(L36:L45)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M46" s="174" t="e">
@@ -25265,11 +27212,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K57" s="171" t="e">
-        <f t="shared" ref="K57" si="10">AVERAGE(K47:K56)</f>
+        <f>AVERAGE(K47:K56)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L57" s="6" t="e">
-        <f t="shared" ref="L57" si="11">AVERAGE(L47:L56)</f>
+        <f>AVERAGE(L47:L56)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M57" s="174" t="e">
@@ -25442,11 +27389,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K68" s="171" t="e">
-        <f t="shared" ref="K68" si="12">AVERAGE(K58:K67)</f>
+        <f>AVERAGE(K58:K67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L68" s="6" t="e">
-        <f t="shared" ref="L68" si="13">AVERAGE(L58:L67)</f>
+        <f>AVERAGE(L58:L67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M68" s="174" t="e">
@@ -25619,11 +27566,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K79" s="171" t="e">
-        <f t="shared" ref="K79" si="14">AVERAGE(K69:K78)</f>
+        <f>AVERAGE(K69:K78)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L79" s="6" t="e">
-        <f t="shared" ref="L79" si="15">AVERAGE(L69:L78)</f>
+        <f>AVERAGE(L69:L78)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M79" s="174" t="e">
@@ -25798,11 +27745,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K90" s="171" t="e">
-        <f t="shared" ref="K90" si="16">AVERAGE(K80:K89)</f>
+        <f>AVERAGE(K80:K89)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L90" s="6" t="e">
-        <f t="shared" ref="L90" si="17">AVERAGE(L80:L89)</f>
+        <f>AVERAGE(L80:L89)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M90" s="174" t="e">
@@ -26757,7 +28704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD356"/>
   <sheetViews>
@@ -42271,7 +44218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD310"/>
   <sheetViews>
@@ -52807,7 +54754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T401"/>
   <sheetViews>
@@ -55769,375 +57716,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="A13:M13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="177" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="179" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="187" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="189"/>
-      <c r="J1" s="181" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="181"/>
-      <c r="L1" s="182"/>
-      <c r="M1" s="183"/>
-    </row>
-    <row r="2" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="178"/>
-      <c r="B2" s="180"/>
-      <c r="C2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="184"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I3" s="29">
-        <v>100</v>
-      </c>
-      <c r="J3" s="14">
-        <v>26418.6422233581</v>
-      </c>
-      <c r="K3" s="43">
-        <f>J3/3600</f>
-        <v>7.338511728710583</v>
-      </c>
-      <c r="L3" s="12">
-        <v>5.2729729219104403E-3</v>
-      </c>
-      <c r="M3" s="27"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I4" s="29">
-        <v>100</v>
-      </c>
-      <c r="J4" s="14">
-        <v>26503.885266065499</v>
-      </c>
-      <c r="K4" s="43">
-        <f>J4/3600</f>
-        <v>7.3621903516848608</v>
-      </c>
-      <c r="L4" s="12">
-        <v>3.1623405133801201E-3</v>
-      </c>
-      <c r="M4" s="21"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I5" s="29">
-        <v>100</v>
-      </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="43">
-        <f t="shared" ref="K5:K12" si="0">J5/3600</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="21"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I6" s="29">
-        <v>100</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I7" s="29">
-        <v>100</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I8" s="29">
-        <v>100</v>
-      </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="21"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I9" s="29">
-        <v>100</v>
-      </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="21"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I10" s="29">
-        <v>100</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="21"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I11" s="29">
-        <v>100</v>
-      </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="21"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11">
-        <v>2000</v>
-      </c>
-      <c r="I12" s="29">
-        <v>100</v>
-      </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="21"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6">
-        <f>AVERAGE(J3:J12)</f>
-        <v>26461.2637447118</v>
-      </c>
-      <c r="K13" s="44">
-        <f>J13/3600</f>
-        <v>7.3503510401977223</v>
-      </c>
-      <c r="L13" s="19">
-        <f>AVERAGE(L3:L12)</f>
-        <v>4.2176567176452802E-3</v>
-      </c>
-      <c r="M13" s="147">
-        <f>_xlfn.STDEV.P(L3:L12)</f>
-        <v>1.0553162042651601E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:M2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>